<commit_message>
Added platform bug to bug log
</commit_message>
<xml_diff>
--- a/Non-Game-Files/BugLog_JumpStreet_TheCrusaders.xlsx
+++ b/Non-Game-Files/BugLog_JumpStreet_TheCrusaders.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SWE0330\Documents\GitHub\JumpyStreetSGD285\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SWE0330\Documents\GitHub\JumpyStreetSGD285\Non-Game-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{865551D4-3D21-4A2C-8226-6E83FB615F62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AC6EC8-8DCB-4FE1-995E-FCC4B842D587}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Issue #</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>spawn map</t>
+  </si>
+  <si>
+    <t>Brennan</t>
+  </si>
+  <si>
+    <t>When jumping sometimes on a platform, usually the player will die when they should not.</t>
+  </si>
+  <si>
+    <t>move left or right while on a platform.</t>
   </si>
 </sst>
 </file>
@@ -829,7 +838,7 @@
   <dimension ref="A1:M258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,14 +913,30 @@
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
+      <c r="G3" s="17">
+        <v>2</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>27</v>
+      </c>
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>

</xml_diff>

<commit_message>
Updated Schedule and bug log
</commit_message>
<xml_diff>
--- a/Non-Game-Files/BugLog_JumpStreet_TheCrusaders.xlsx
+++ b/Non-Game-Files/BugLog_JumpStreet_TheCrusaders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SWE0330\Documents\GitHub\JumpyStreetSGD285\Non-Game-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AC6EC8-8DCB-4FE1-995E-FCC4B842D587}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CBB7A6-11CF-4900-AD60-11AEAD3E0593}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Issue #</t>
   </si>
@@ -160,10 +160,22 @@
     <t>Brennan</t>
   </si>
   <si>
-    <t>When jumping sometimes on a platform, usually the player will die when they should not.</t>
-  </si>
-  <si>
-    <t>move left or right while on a platform.</t>
+    <t>At a certain point in progression the player is often bumped back a tile by the model somehow trying to progress further than it is recorded to have progressed.</t>
+  </si>
+  <si>
+    <t>Move forward enough</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>move on a platform</t>
+  </si>
+  <si>
+    <t>When jumping on a log the player slowly acends into the air.</t>
   </si>
 </sst>
 </file>
@@ -838,7 +850,7 @@
   <dimension ref="A1:M258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,7 +925,7 @@
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
     </row>
-    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -921,10 +933,10 @@
         <v>43</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -935,21 +947,37 @@
         <v>21</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
+      <c r="G4" s="17">
+        <v>4</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>

</xml_diff>